<commit_message>
Changed frac MAM to SAM & SAM to MAM to 1, updated so that unrestrictedCov is used
</commit_message>
<xml_diff>
--- a/Projects/Master/data/national/InputForCode_Master.xlsx
+++ b/Projects/Master/data/national/InputForCode_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/Projects/Master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D00450D1-E537-7B43-84E2-175B9B807AD1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{41C1A269-BD93-F241-9067-0DFFB85EFA65}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="17" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2971,7 +2971,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="271">
   <si>
     <t>year</t>
   </si>
@@ -7340,8 +7340,8 @@
   </sheetPr>
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A3" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7450,7 +7450,7 @@
         <v>210</v>
       </c>
       <c r="C12" s="130">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -7458,7 +7458,7 @@
         <v>211</v>
       </c>
       <c r="C13" s="130">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -8188,8 +8188,8 @@
   </sheetPr>
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8454,7 +8454,9 @@
       <c r="A41" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B41" s="98"/>
+      <c r="B41" s="98" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
@@ -9427,8 +9429,8 @@
   </sheetPr>
   <dimension ref="A1:Y103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13243,11 +13245,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -13258,6 +13255,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -18126,7 +18128,7 @@
   </sheetPr>
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>